<commit_message>
Debugged and Fixed NullPointerException
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -1,25 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohai\IdeaProjects\Assignment_Q1\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9BED46-19B0-46CC-92DA-069583976FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet state="visible" name="Saturday" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sunday" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Monday" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Tuesday" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Wednesday" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Thursday" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Friday" sheetId="7" r:id="rId10"/>
+    <sheet name="Saturday" sheetId="1" r:id="rId1"/>
+    <sheet name="Sunday" sheetId="2" r:id="rId2"/>
+    <sheet name="Monday" sheetId="3" r:id="rId3"/>
+    <sheet name="Tuesday" sheetId="4" r:id="rId4"/>
+    <sheet name="Wednesday" sheetId="5" r:id="rId5"/>
+    <sheet name="Thursday" sheetId="6" r:id="rId6"/>
+    <sheet name="Friday" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="57">
   <si>
     <t>Longest Option</t>
   </si>
@@ -110,16 +117,10 @@
 মাধ্যমিক ও উচ্চমাধ্যমিক শিক্ষা বোর্ড, ঢাকা · ঢাকা</t>
   </si>
   <si>
-    <t>dhaka888</t>
-  </si>
-  <si>
     <t>Saturday Night Live
 স্যাটারডে নাইট লাইভ — টিভি প্রোগ্রাম</t>
   </si>
   <si>
-    <t>dhaka post</t>
-  </si>
-  <si>
     <t>BABYMONSTER
 বেবি মনস্টার — মিউজিক্যাল গ্রুপ</t>
   </si>
@@ -148,10 +149,6 @@
     <t>cricket</t>
   </si>
   <si>
-    <t>inter milan
-ইন্টার মিলান — ফুটবল টীম</t>
-  </si>
-  <si>
     <t>money</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
 লুক চেঞ্জ লাইফস্টাইল স্যালুন · ঢাকা</t>
   </si>
   <si>
-    <t>লগইন</t>
-  </si>
-  <si>
     <t>Hello Hello! (Noodle &amp; Pals) [Sing-Along]
 গান</t>
   </si>
@@ -169,46 +163,71 @@
     <t>look</t>
   </si>
   <si>
+    <t>dhaka 888</t>
+  </si>
+  <si>
+    <t>interrogative sentence কাকে বলে</t>
+  </si>
+  <si>
     <t>বয়স্ক ভাতা আবেদন অনলাইন 2025</t>
   </si>
   <si>
-    <t>ভিসা</t>
-  </si>
-  <si>
-    <t>l89</t>
-  </si>
-  <si>
-    <t>dhaka 888</t>
-  </si>
-  <si>
-    <t>ঢাকা পোস্ট</t>
+    <t>dhaka post</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>লোকেশন</t>
+  </si>
+  <si>
+    <t>Inter Miami
+ইন্টার মায়ামি সিএফ — ফুটবল টীম</t>
+  </si>
+  <si>
+    <t>look change lifestyle salon uttara</t>
+  </si>
+  <si>
+    <t>babu88</t>
+  </si>
+  <si>
+    <t>pathao office near me</t>
+  </si>
+  <si>
+    <t>pathao food</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>ইন্টারনেট</t>
   </si>
   <si>
-    <t>mom and son
-Mother and Son — ২০২২ সালের চলচ্চিত্র</t>
+    <t>ind vs nz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -219,11 +238,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -237,59 +262,37 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -479,11 +482,179 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="B2:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:5" ht="28" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -491,9 +662,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:5" ht="28" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,153 +672,93 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4">
+    </row>
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6">
+    </row>
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7">
+    </row>
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8">
+    </row>
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9">
+    </row>
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10">
+    </row>
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11">
+    </row>
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s" s="0">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12">
+    </row>
+    <row r="12" spans="2:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s" s="0">
-        <v>46</v>
-      </c>
-      <c r="E12" t="s" s="0">
-        <v>47</v>
-      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -655,9 +766,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:5" ht="28" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,7 +776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -673,15 +784,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -689,7 +800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -697,7 +808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -705,7 +816,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -713,7 +824,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -721,7 +832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -729,7 +840,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -737,7 +848,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="2:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
@@ -746,12 +857,12 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -759,9 +870,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:5" ht="28" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -769,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -777,15 +888,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -793,7 +904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -801,7 +912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -809,7 +920,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -817,7 +928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -825,15 +936,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -841,7 +952,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="2:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
@@ -850,12 +961,178 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="B2:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:5" ht="28" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -863,9 +1140,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:5" ht="28" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,7 +1150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -881,7 +1158,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -889,7 +1166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -897,7 +1174,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -905,7 +1182,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -913,7 +1190,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -921,7 +1198,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -929,15 +1206,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -945,7 +1222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="2:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
@@ -954,12 +1231,12 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -967,223 +1244,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="2">
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="B2:E12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="2">
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="B2:E12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" customWidth="true" width="10.13"/>
-    <col min="4" max="4" customWidth="true" width="8.13"/>
-    <col min="5" max="5" customWidth="true" width="8.25"/>
+    <col min="2" max="3" customWidth="true" width="10.08984375"/>
+    <col min="4" max="4" customWidth="true" width="8.08984375"/>
+    <col min="5" max="5" customWidth="true" width="8.26953125"/>
     <col min="6" max="6" customWidth="true" width="5.0"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:5" ht="28" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1199,7 +1268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1207,7 +1276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1215,7 +1284,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1223,7 +1292,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1231,7 +1300,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1239,7 +1308,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1247,7 +1316,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1255,7 +1324,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -1263,7 +1332,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="2:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1272,6 +1341,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>